<commit_message>
Finished EP24 Promotion | Graph
</commit_message>
<xml_diff>
--- a/firstweb/order_menu_data.xlsx
+++ b/firstweb/order_menu_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -873,6 +873,45 @@
         <v>27.79</v>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Hawailian</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>30</v>
+      </c>
+      <c r="C19" t="n">
+        <v>7624.5</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Iced Cappucino</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>15</v>
+      </c>
+      <c r="C20" t="n">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Iced Amercano</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>1</v>
+      </c>
+      <c r="C21" t="n">
+        <v>49</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>